<commit_message>
Import Config from Excel
</commit_message>
<xml_diff>
--- a/.init/permits.xlsx
+++ b/.init/permits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Coding\django-yolobuilds\.init\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A8684F-9599-4940-B5B1-4428E6D3AFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41D86A6-A783-4C40-8BF9-8FA6727FCE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12228" yWindow="252" windowWidth="10812" windowHeight="12252" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sequence" sheetId="4" r:id="rId1"/>
@@ -1389,9 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{458F1381-84CA-4D75-874A-529E18BFB144}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1509,7 +1507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6F4446-BD57-4EC8-856F-43841E10407C}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>61</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>59</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>57</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>55</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>53</v>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>51</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>49</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>47</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>45</v>
@@ -1641,7 +1641,7 @@
   <dimension ref="A1:R144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>38</v>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>501</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>36</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>502</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>34</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>503</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>32</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>504</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>30</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>505</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>28</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>506</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>26</v>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>507</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>24</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>508</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>22</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>509</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>20</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>510</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>511</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>16</v>
@@ -2302,7 +2302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F8B687-30FE-4759-985F-258ED83A1BFE}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2364,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747E8157-706F-4F14-9408-4AA2AE28E2A0}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>